<commit_message>
added excel database for boards
</commit_message>
<xml_diff>
--- a/data/board-database.xlsx
+++ b/data/board-database.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56710FA7-9127-4CC1-B352-050BE70238CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{760066AE-1076-42BB-9730-14F8A5892F97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,12 +76,6 @@
     <t>pappy-board.jpg</t>
   </si>
   <si>
-    <t>Image front</t>
-  </si>
-  <si>
-    <t>Image back</t>
-  </si>
-  <si>
     <t>board3-back.jpg</t>
   </si>
   <si>
@@ -107,6 +101,12 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>ImageFront</t>
+  </si>
+  <si>
+    <t>ImageBack</t>
   </si>
 </sst>
 </file>
@@ -174,8 +174,8 @@
     <tableColumn id="2" xr3:uid="{9C7EB252-219C-4037-BBD3-D8391EF0AA30}" name="Title"/>
     <tableColumn id="3" xr3:uid="{6BDDEA68-A924-4A86-BE23-B642EEBC3913}" name="Description"/>
     <tableColumn id="4" xr3:uid="{E362BD63-9A83-443C-85AC-8C92F0E4A3DF}" name="Price"/>
-    <tableColumn id="5" xr3:uid="{0FF80485-6C94-4A84-A33F-B4458B7E8E94}" name="Image front"/>
-    <tableColumn id="6" xr3:uid="{C8CD7A07-1CCA-4C72-96DF-3E65E4C92DE9}" name="Image back"/>
+    <tableColumn id="5" xr3:uid="{0FF80485-6C94-4A84-A33F-B4458B7E8E94}" name="ImageFront"/>
+    <tableColumn id="6" xr3:uid="{C8CD7A07-1CCA-4C72-96DF-3E65E4C92DE9}" name="ImageBack"/>
     <tableColumn id="7" xr3:uid="{70EDF6EC-D346-4CC8-A34B-586155E42F8D}" name="Display"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -522,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -562,7 +562,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -570,22 +570,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -593,19 +593,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>